<commit_message>
Adde crude controller and helper files, tons of other stuff why didnt i do this sooner
</commit_message>
<xml_diff>
--- a/PDM_integration/parameters.xlsx
+++ b/PDM_integration/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anigo\OneDrive\Documents\GitHub\Modeling-and-control\PDM_integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89115632-8F47-4A39-8F63-EA8DA837F47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E070F4-5012-4012-A0D0-99FBCB75FB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -392,7 +392,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -408,7 +408,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a bunch of files
</commit_message>
<xml_diff>
--- a/PDM_integration/parameters.xlsx
+++ b/PDM_integration/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anigo\OneDrive\Documents\GitHub\Modeling-and-control\PDM_integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E070F4-5012-4012-A0D0-99FBCB75FB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9793262-D77C-48AB-93E8-E62DDC304088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,7 +354,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -364,7 +364,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -378,7 +378,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -392,7 +392,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated a bunch of controller stuff, still a work-in-progress
</commit_message>
<xml_diff>
--- a/PDM_integration/parameters.xlsx
+++ b/PDM_integration/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anigo\OneDrive\Documents\GitHub\Modeling-and-control\PDM_integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9793262-D77C-48AB-93E8-E62DDC304088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1638BD96-CFBE-400E-AE6A-ADBD3CE636DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,7 +354,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Interim post-overhaul commit for embedded coder
</commit_message>
<xml_diff>
--- a/PDM_integration/parameters.xlsx
+++ b/PDM_integration/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anigo\OneDrive\Documents\GitHub\Modeling-and-control\PDM_integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C25DF6-0743-4007-89C0-E4ACCAE283E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA93D17-F3D4-42FF-B3CD-A8C0AD846405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +355,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -364,35 +365,35 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.01</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>-8.8800000000000004E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <v>0.55179999999999996</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>9.7345000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" s="1">
+        <v>-8.8800000000000004E-2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>9.7345000000000001E-2</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>4.2318000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed MOI matrix - WARNING: the program will not work very well if you don't have realistic values for constants (m, g, l, MOI)
</commit_message>
<xml_diff>
--- a/PDM_integration/parameters.xlsx
+++ b/PDM_integration/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anigo\OneDrive\Documents\GitHub\Modeling-and-control\PDM_integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6CD517-2FAE-4A71-B4CB-1F25D528638C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA93D17-F3D4-42FF-B3CD-A8C0AD846405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +355,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -364,35 +365,35 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>100</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>-8.8800000000000004E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" s="1">
+        <v>2.3E-2</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>0.55179999999999996</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>9.7345000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" s="1">
+        <v>-8.8800000000000004E-2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>9.7345000000000001E-2</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>4.2318000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>